<commit_message>
updated OpenIMU330 pinout description
</commit_message>
<xml_diff>
--- a/330BI/_docs/OpenIMU330BI_Pin_Definition.xlsx
+++ b/330BI/_docs/OpenIMU330BI_Pin_Definition.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -77,10 +77,6 @@
   </si>
   <si>
     <t>No.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -493,6 +489,57 @@
       </rPr>
       <t>I/O</t>
     </r>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>MCU Pin</t>
+  </si>
+  <si>
+    <t>PB11</t>
+  </si>
+  <si>
+    <t>PB10</t>
+  </si>
+  <si>
+    <t>PA11</t>
+  </si>
+  <si>
+    <t>PA9</t>
+  </si>
+  <si>
+    <t>NRST</t>
+  </si>
+  <si>
+    <t>PA10</t>
+  </si>
+  <si>
+    <t>PB14</t>
+  </si>
+  <si>
+    <t>PB13</t>
+  </si>
+  <si>
+    <t>PA13</t>
+  </si>
+  <si>
+    <t>PB3</t>
+  </si>
+  <si>
+    <t>PB5</t>
+  </si>
+  <si>
+    <t>PH3</t>
+  </si>
+  <si>
+    <t>PA14</t>
+  </si>
+  <si>
+    <t>PA12</t>
+  </si>
+  <si>
+    <t>PB15</t>
   </si>
 </sst>
 </file>
@@ -554,7 +601,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -691,28 +738,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -739,6 +808,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,13 +853,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>39283</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>185056</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>549823</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>6152</xdr:rowOff>
@@ -1103,675 +1196,754 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="4" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="9" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.25" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" ht="17.25" thickBot="1">
+      <c r="A1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
+      <c r="G1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="5" t="s">
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="C33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="8" t="s">
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="E36" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="D42" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="11" t="s">
+    <row r="43" spans="1:5">
+      <c r="A43" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="11" t="s">
+      <c r="E44" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="17"/>
+      <c r="C45" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" s="14" t="s">
+      <c r="E45" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:O1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:P1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated OpenIMU330 title in pin description file
</commit_message>
<xml_diff>
--- a/330BI/_docs/OpenIMU330BI_Pin_Definition.xlsx
+++ b/330BI/_docs/OpenIMU330BI_Pin_Definition.xlsx
@@ -311,10 +311,6 @@
   </si>
   <si>
     <t>GPIO2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OpenIMU330BI module top view of package</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -540,6 +536,9 @@
   </si>
   <si>
     <t>PB15</t>
+  </si>
+  <si>
+    <t>OpenIMU330BI module bottom view of package</t>
   </si>
 </sst>
 </file>
@@ -808,7 +807,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -821,15 +829,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1198,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5"/>
@@ -1213,35 +1212,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17.25" thickBot="1">
-      <c r="A1" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
-      <c r="G1" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="G1" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>101</v>
+      <c r="B2" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>16</v>
@@ -1254,7 +1253,7 @@
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
@@ -1269,7 +1268,7 @@
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1284,7 +1283,7 @@
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="17"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1299,7 +1298,7 @@
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1314,7 +1313,7 @@
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
@@ -1329,7 +1328,7 @@
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
@@ -1344,7 +1343,7 @@
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="17"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
@@ -1359,7 +1358,7 @@
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="6" t="s">
         <v>2</v>
       </c>
@@ -1374,7 +1373,7 @@
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
@@ -1389,7 +1388,7 @@
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="6" t="s">
         <v>2</v>
       </c>
@@ -1404,7 +1403,7 @@
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
@@ -1419,8 +1418,8 @@
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>102</v>
+      <c r="B14" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>14</v>
@@ -1429,15 +1428,15 @@
         <v>9</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>103</v>
+      <c r="B15" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>13</v>
@@ -1446,14 +1445,14 @@
         <v>8</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="6" t="s">
         <v>66</v>
       </c>
@@ -1468,7 +1467,7 @@
       <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="6" t="s">
         <v>2</v>
       </c>
@@ -1483,7 +1482,7 @@
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="6" t="s">
         <v>64</v>
       </c>
@@ -1491,14 +1490,14 @@
         <v>65</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="17"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="6" t="s">
         <v>2</v>
       </c>
@@ -1513,7 +1512,7 @@
       <c r="A20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="6" t="s">
         <v>64</v>
       </c>
@@ -1521,14 +1520,14 @@
         <v>65</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="6" t="s">
         <v>2</v>
       </c>
@@ -1543,7 +1542,7 @@
       <c r="A22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="17"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="6" t="s">
         <v>64</v>
       </c>
@@ -1551,14 +1550,14 @@
         <v>65</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="17"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="6" t="s">
         <v>2</v>
       </c>
@@ -1573,25 +1572,25 @@
       <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>104</v>
+      <c r="B24" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>69</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>105</v>
+      <c r="B25" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>63</v>
@@ -1600,15 +1599,15 @@
         <v>8</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>106</v>
+      <c r="B26" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>70</v>
@@ -1617,14 +1616,14 @@
         <v>62</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="6" t="s">
         <v>2</v>
       </c>
@@ -1639,7 +1638,7 @@
       <c r="A28" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="6" t="s">
         <v>2</v>
       </c>
@@ -1654,7 +1653,7 @@
       <c r="A29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="6" t="s">
         <v>2</v>
       </c>
@@ -1669,7 +1668,7 @@
       <c r="A30" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="17"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="6" t="s">
         <v>71</v>
       </c>
@@ -1677,32 +1676,32 @@
         <v>10</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>116</v>
+      <c r="B31" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>107</v>
+      <c r="B32" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>72</v>
@@ -1711,14 +1710,14 @@
         <v>9</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="17"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="6" t="s">
         <v>64</v>
       </c>
@@ -1726,15 +1725,15 @@
         <v>65</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="17" t="s">
-        <v>108</v>
+      <c r="B34" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>73</v>
@@ -1743,15 +1742,15 @@
         <v>8</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="17" t="s">
-        <v>109</v>
+      <c r="B35" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>74</v>
@@ -1760,14 +1759,14 @@
         <v>9</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="17"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="6" t="s">
         <v>2</v>
       </c>
@@ -1782,8 +1781,8 @@
       <c r="A37" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>110</v>
+      <c r="B37" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>4</v>
@@ -1792,31 +1791,31 @@
         <v>1</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="17" t="s">
-        <v>111</v>
+      <c r="B38" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="17"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="6" t="s">
         <v>64</v>
       </c>
@@ -1824,14 +1823,14 @@
         <v>65</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="17"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="6" t="s">
         <v>64</v>
       </c>
@@ -1839,21 +1838,21 @@
         <v>65</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>112</v>
+      <c r="B41" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>75</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>7</v>
@@ -1863,7 +1862,7 @@
       <c r="A42" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="17"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="6" t="s">
         <v>2</v>
       </c>
@@ -1878,25 +1877,25 @@
       <c r="A43" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="17" t="s">
-        <v>113</v>
+      <c r="B43" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>76</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="17" t="s">
-        <v>114</v>
+      <c r="B44" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>5</v>
@@ -1912,7 +1911,7 @@
       <c r="A45" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="17"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="6" t="s">
         <v>64</v>
       </c>
@@ -1920,24 +1919,24 @@
         <v>65</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="17" t="s">
-        <v>115</v>
+      <c r="B46" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>77</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>